<commit_message>
Updated the Integration plan to combine integration step 9-11 into 1. Implemented the new step 9 of the integration plan.
</commit_message>
<xml_diff>
--- a/IntegrationPlan.xlsx
+++ b/IntegrationPlan.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjark\source\repos\MicrowaveHandin3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mikkel\Documents\6_semester\SWT\MicrowaveHandin3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A481463A-D9D3-4CCA-9894-50F183BCF875}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00962995-CB7A-4AA3-A9AE-C03877C031E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32175" yWindow="3375" windowWidth="21600" windowHeight="11385" xr2:uid="{C786DE82-1E2F-47BD-B35B-9FFE731C1056}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C786DE82-1E2F-47BD-B35B-9FFE731C1056}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="13">
   <si>
     <t>UI</t>
   </si>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -423,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D73304DD-F36F-4380-9C0F-04BE678019DF}">
-  <dimension ref="B2:K13"/>
+  <dimension ref="B2:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
@@ -709,79 +709,15 @@
         <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J11" t="s">
         <v>11</v>
       </c>
       <c r="K11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>